<commit_message>
Thay đổi dữ liệu điểm phân hóa sinh viên hơn
</commit_message>
<xml_diff>
--- a/resources/database/classes.xlsx
+++ b/resources/database/classes.xlsx
@@ -250,73 +250,6 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <fgColor indexed="64"/>
@@ -408,6 +341,73 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -422,12 +422,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C25" totalsRowShown="0" headerRowDxfId="0" dataDxfId="4" headerRowBorderDxfId="2" tableBorderDxfId="3" totalsRowBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C25" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A1:C25"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="MLH" dataDxfId="7"/>
-    <tableColumn id="2" name="Học Kì" dataDxfId="6"/>
-    <tableColumn id="3" name="Tên" dataDxfId="5"/>
+    <tableColumn id="1" name="MLH" dataDxfId="2"/>
+    <tableColumn id="2" name="Học Kì" dataDxfId="1"/>
+    <tableColumn id="3" name="Tên" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -706,7 +706,7 @@
   <cols>
     <col min="1" max="1" width="17" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -874,7 +874,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>38</v>
       </c>
@@ -907,7 +907,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>41</v>
       </c>
@@ -918,7 +918,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Điều chỉnh dữ liệu, tăng số lượng kỳ học lên 7, phân hóa bằng cách sinh viên các kỳ sau học môn khác nhau theo nhóm
</commit_message>
<xml_diff>
--- a/resources/database/classes.xlsx
+++ b/resources/database/classes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="124">
   <si>
     <t>MLH</t>
   </si>
@@ -172,6 +172,225 @@
   </si>
   <si>
     <t>INT2208</t>
+  </si>
+  <si>
+    <t>HIS1001</t>
+  </si>
+  <si>
+    <t>POL1001</t>
+  </si>
+  <si>
+    <t>Lịch sử Đảng Cộng sản Việt Nam</t>
+  </si>
+  <si>
+    <t>Tư tưởng Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Nguyên lý hệ điều hành</t>
+  </si>
+  <si>
+    <t>INT3131</t>
+  </si>
+  <si>
+    <t>INT3132</t>
+  </si>
+  <si>
+    <t>INT3401</t>
+  </si>
+  <si>
+    <t>INT3507</t>
+  </si>
+  <si>
+    <t>INT3508</t>
+  </si>
+  <si>
+    <t>Dự án khoa học</t>
+  </si>
+  <si>
+    <t>Dự án công nghệ</t>
+  </si>
+  <si>
+    <t>Trí tuệ nhân tạo</t>
+  </si>
+  <si>
+    <t>Các vấn đề hiện đại của CNTT</t>
+  </si>
+  <si>
+    <t>Thực tập chuyên ngành</t>
+  </si>
+  <si>
+    <t>INT3117</t>
+  </si>
+  <si>
+    <t>INT3105</t>
+  </si>
+  <si>
+    <t>INT3106</t>
+  </si>
+  <si>
+    <t>INT3108</t>
+  </si>
+  <si>
+    <t>INT3109</t>
+  </si>
+  <si>
+    <t>INT3111</t>
+  </si>
+  <si>
+    <t>INT3115</t>
+  </si>
+  <si>
+    <t>INT3120</t>
+  </si>
+  <si>
+    <t>INT3306</t>
+  </si>
+  <si>
+    <t>INT3110</t>
+  </si>
+  <si>
+    <t>Kiểm thử và đảm bảo chất lượng phần mềm</t>
+  </si>
+  <si>
+    <t>Kiến trúc phần mềm</t>
+  </si>
+  <si>
+    <t>Phương pháp hình thức</t>
+  </si>
+  <si>
+    <t>Lập trình nhúng và thời gian thực</t>
+  </si>
+  <si>
+    <t>Thu thập và phân tích yêu cầu</t>
+  </si>
+  <si>
+    <t>Quản lý dự án phần mềm</t>
+  </si>
+  <si>
+    <t>Thiết kế giao diện người dùng</t>
+  </si>
+  <si>
+    <t>Phát triển ứng dụng di động</t>
+  </si>
+  <si>
+    <t>Phát triển ứng dụng Web</t>
+  </si>
+  <si>
+    <t>Phân tích và thiết kế hướng đối tượng</t>
+  </si>
+  <si>
+    <t>INT3202</t>
+  </si>
+  <si>
+    <t>INT3209</t>
+  </si>
+  <si>
+    <t>INT3225</t>
+  </si>
+  <si>
+    <t>INT3229</t>
+  </si>
+  <si>
+    <t>INT3230</t>
+  </si>
+  <si>
+    <t>INT3228</t>
+  </si>
+  <si>
+    <t>INT2020</t>
+  </si>
+  <si>
+    <t>INT3505</t>
+  </si>
+  <si>
+    <t>INT3506</t>
+  </si>
+  <si>
+    <t>INT3501</t>
+  </si>
+  <si>
+    <t>Hệ quản trị cơ sở dữ liệu</t>
+  </si>
+  <si>
+    <t>Khai phá dữ liệu</t>
+  </si>
+  <si>
+    <t>Trí tuệ kinh doanh</t>
+  </si>
+  <si>
+    <t>Kỹ thuật và công nghệ dữ liệu lớn</t>
+  </si>
+  <si>
+    <t>Mật mã và an toàn thông tin</t>
+  </si>
+  <si>
+    <t>Thiết kế và phân tích thực nghiệm</t>
+  </si>
+  <si>
+    <t>Phân tích thiết kế các HTTT</t>
+  </si>
+  <si>
+    <t>Kiến trúc hướng dịch vụ</t>
+  </si>
+  <si>
+    <t>Các hệ thống thương mại điện tử</t>
+  </si>
+  <si>
+    <t>Khoa học dịch vụ</t>
+  </si>
+  <si>
+    <t>INT3404</t>
+  </si>
+  <si>
+    <t>INT3423</t>
+  </si>
+  <si>
+    <t>INT3422</t>
+  </si>
+  <si>
+    <t>INT3402</t>
+  </si>
+  <si>
+    <t>INT3405</t>
+  </si>
+  <si>
+    <t>INT3406</t>
+  </si>
+  <si>
+    <t>Xử lý ảnh</t>
+  </si>
+  <si>
+    <t>Tin sinh học ứng dụng</t>
+  </si>
+  <si>
+    <t>Tin học y tế</t>
+  </si>
+  <si>
+    <t>Chương trình dịch</t>
+  </si>
+  <si>
+    <t>Học máy</t>
+  </si>
+  <si>
+    <t>Xử lý ngôn ngữ tự nhiên</t>
+  </si>
+  <si>
+    <t>UET1002</t>
+  </si>
+  <si>
+    <t>INT3418</t>
+  </si>
+  <si>
+    <t>INT3102</t>
+  </si>
+  <si>
+    <t>Kỹ năng khởi nghiệp</t>
+  </si>
+  <si>
+    <t>Thuật toán nâng cao và ứng dụng</t>
+  </si>
+  <si>
+    <t>Phương pháp tính</t>
   </si>
 </sst>
 </file>
@@ -187,13 +406,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +422,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -234,15 +489,60 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -250,13 +550,57 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill>
           <fgColor indexed="64"/>
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -267,6 +611,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -291,7 +641,7 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -304,6 +654,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -328,7 +684,7 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -339,44 +695,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -388,8 +712,6 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
       </font>
       <fill>
         <patternFill>
@@ -397,15 +719,35 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top/>
-        <bottom/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -422,12 +764,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C25" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:C25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C62" totalsRowShown="0" headerRowDxfId="0" dataDxfId="4" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:C62"/>
+  <sortState ref="A2:C62">
+    <sortCondition ref="B1:B62"/>
+  </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="MLH" dataDxfId="2"/>
-    <tableColumn id="2" name="Học Kì" dataDxfId="1"/>
-    <tableColumn id="3" name="Tên" dataDxfId="0"/>
+    <tableColumn id="1" name="MLH" dataDxfId="3"/>
+    <tableColumn id="2" name="Học Kì" dataDxfId="2"/>
+    <tableColumn id="3" name="Tên" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -696,292 +1041,700 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.109375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="9">
         <v>2</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="9">
         <v>2</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="9">
         <v>2</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="9">
         <v>2</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="9">
         <v>2</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="16">
         <v>3</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="16">
         <v>3</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="16">
         <v>3</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="16">
         <v>3</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="16">
         <v>3</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="16">
         <v>3</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="6">
         <v>4</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="6">
         <v>4</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="6">
         <v>4</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="6">
         <v>4</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="6">
         <v>4</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="6">
         <v>4</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="7" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="13">
+        <v>5</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="13">
+        <v>5</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="13">
+        <v>5</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="13">
+        <v>5</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="13">
+        <v>5</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="13">
+        <v>5</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="13">
+        <v>5</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="13">
+        <v>5</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="13" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="13">
+        <v>5</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="13">
+        <v>5</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="13">
+        <v>5</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="11">
+        <v>6</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="11">
+        <v>6</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="11">
+        <v>6</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="11">
+        <v>6</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="11">
+        <v>6</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="11">
+        <v>6</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="11" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" s="11">
+        <v>6</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="11">
+        <v>6</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" s="11">
+        <v>6</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" s="11">
+        <v>6</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="11">
+        <v>6</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="11">
+        <v>6</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B49" s="11">
+        <v>6</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B50" s="11">
+        <v>6</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B51" s="11">
+        <v>6</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" s="13">
+        <v>7</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="13">
+        <v>7</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B54" s="13">
+        <v>7</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B55" s="13">
+        <v>7</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B56" s="13">
+        <v>7</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B57" s="13">
+        <v>7</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B58" s="13">
+        <v>7</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B59" s="13">
+        <v>7</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B60" s="13">
+        <v>7</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B61" s="13">
+        <v>7</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B62" s="13">
+        <v>7</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>